<commit_message>
6 Apr commit 1
</commit_message>
<xml_diff>
--- a/client/public/assets/Create Tasks.xlsx
+++ b/client/public/assets/Create Tasks.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10402"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2084CA3C-AAE2-C547-AD48-C0AEA4BFFF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="22260" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,16 +43,16 @@
     <t>Sprint</t>
   </si>
   <si>
-    <t>Start Date (dd-mm-yyyy)</t>
-  </si>
-  <si>
-    <t>Due Date (dd-mm-yyyy)</t>
+    <t>Start Date (dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t>Due Date (dd/mm/yyyy)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,26 +372,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
-    <col min="5" max="5" width="25.81640625" customWidth="1"/>
-    <col min="6" max="6" width="24.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="8" width="15.08984375" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -421,7 +422,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Urgent, High, Medium, Low, Backlog"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>